<commit_message>
Now I have figured out how they generated all the combinations of 3
</commit_message>
<xml_diff>
--- a/CH-101 Subsets.xlsx
+++ b/CH-101 Subsets.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65BEDD3-3250-4175-AC26-C6C5D6CF4E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7073CBD-5DC0-4E6C-9D73-D66DF6E28261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -253,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +283,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -329,6 +332,121 @@
         <a:xfrm>
           <a:off x="2286000" y="19050"/>
           <a:ext cx="2486025" cy="2400300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:alpha val="88000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="freezing" dir="t"/>
+        </a:scene3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="2000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Challenge 101: Subsets</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="2000" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="2000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Extract the subset of ID combinations consisting of 3 members, along with their total cost.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="2000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5AF5A06-763F-45F8-B42E-9795E44576E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2124075" y="19050"/>
+          <a:ext cx="2263140" cy="2266950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -649,7 +767,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="802" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="9">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -665,6 +783,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1252,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6000F1B7-4689-4742-BD98-C75A541BB8E6}">
   <dimension ref="B1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,7 +1646,10 @@
       <c r="E19" s="1" t="str">
         <v>1</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="str" cm="1">
+        <f t="array" ref="F19:F28">_xlfn._xlws.FILTER(E19:E49,LEN(E19:E49)=5)</f>
+        <v>1,2,3</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -1539,7 +1663,9 @@
       <c r="E20" s="1" t="str">
         <v>2</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="str">
+        <v>1,2,4</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -1553,7 +1679,9 @@
       <c r="E21" s="1" t="str">
         <v>1,2</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="str">
+        <v>1,3,4</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -1567,7 +1695,9 @@
       <c r="E22" s="1" t="str">
         <v>3</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="str">
+        <v>2,3,4</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -1581,7 +1711,9 @@
       <c r="E23" s="1" t="str">
         <v>1,3</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="str">
+        <v>1,2,5</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -1595,7 +1727,9 @@
       <c r="E24" s="1" t="str">
         <v>2,3</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="str">
+        <v>1,3,5</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -1609,7 +1743,9 @@
       <c r="E25" s="1" t="str">
         <v>1,2,3</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="str">
+        <v>2,3,5</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -1622,6 +1758,9 @@
       <c r="E26" t="str">
         <v>4</v>
       </c>
+      <c r="F26" t="str">
+        <v>1,4,5</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="str">
@@ -1633,10 +1772,16 @@
       <c r="E27" t="str">
         <v>1,4</v>
       </c>
+      <c r="F27" t="str">
+        <v>2,4,5</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E28" t="str">
         <v>2,4</v>
+      </c>
+      <c r="F28" t="str">
+        <v>3,4,5</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -1752,4 +1897,656 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A5850E-FA09-4AFD-8CA9-0CFA8DE0E538}">
+  <dimension ref="B1:I47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
+    <col min="9" max="9" width="15.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" customWidth="1"/>
+    <col min="12" max="12" width="9.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="H1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10"/>
+      <c r="H10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="15" cm="1">
+        <f t="array" ref="F16:F47">_xlfn.REDUCE(
+0,
+B3:B7,
+_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.LET(_xlpm.db,_xlpm.a&amp;","&amp;_xlpm.v,_xlpm.db)))
+)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="e">
+        <f>_xlfn.TEXTAFTER(F16,",",1)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16:H25">_xlfn._xlws.FILTER(G17:G47,LEN(G17:G47)=5)</f>
+        <v>1,2,3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C17" t="str" cm="1">
+        <f t="array" ref="C17:D26">_xlfn.LET(
+    _xlpm.id, B3:B7,
+    _xlpm.val, C3:C7,
+    _xlpm.genCom, _xlfn.DROP(
+        _xlfn.IFNA(
+            _xlfn.REDUCE(
+                0,
+                _xlfn.DROP(
+                    _xlfn.REDUCE(
+                        0,
+                        B3:B7,
+                        _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.LET(_xlpm.db, _xlpm.a &amp; "," &amp; _xlpm.v, _xlpm.db)))
+                    ),
+                    1
+                ),
+                _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.TEXTSPLIT(_xlpm.v, ",")))
+            ),
+            ""
+        ),
+        1,
+        1
+    ),
+    _xlpm.list3com, _xlfn.DROP(
+        _xlfn._xlws.FILTER(_xlpm.genCom, _xlfn.BYROW(_xlpm.genCom, _xlfn.LAMBDA(_xlpm.r, COUNTA(_xlfn.TOCOL(--_xlpm.r, 2)))) = 3),
+        ,
+        -2
+    ),
+    _xlpm.tc, _xlfn.BYROW(_xlfn.MAP(--_xlpm.list3com, _xlfn.LAMBDA(_xlpm.m, _xlfn.XLOOKUP(_xlpm.m, _xlpm.id, _xlpm.val))), _xlfn.LAMBDA(_xlpm.r, SUM(_xlpm.r))),
+    _xlfn._xlws.SORT(_xlfn.HSTACK(_xlfn.BYROW(_xlpm.list3com, _xlfn.LAMBDA(_xlpm.r, _xlfn.TEXTJOIN(",", , _xlpm.r))), _xlpm.tc), 2, 1)
+)</f>
+        <v>1,2,3</v>
+      </c>
+      <c r="D17" s="14">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="15" t="str">
+        <v>0,1</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" ref="G17:G47" si="0">_xlfn.TEXTAFTER(F17,",",1)</f>
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <v>1,2,4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C18" t="str">
+        <v>1,2,4</v>
+      </c>
+      <c r="D18" s="14">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="15" t="str">
+        <v>0,2</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H18" t="str">
+        <v>1,3,4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <v>1,3,4</v>
+      </c>
+      <c r="D19" s="14">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="15" t="str">
+        <v>0,1,2</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2</v>
+      </c>
+      <c r="H19" t="str">
+        <v>2,3,4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <v>2,3,4</v>
+      </c>
+      <c r="D20" s="14">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="15" t="str">
+        <v>0,3</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H20" t="str">
+        <v>1,2,5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <v>1,2,5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="15" t="str">
+        <v>0,1,3</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,3</v>
+      </c>
+      <c r="H21" t="str">
+        <v>1,3,5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <v>1,3,5</v>
+      </c>
+      <c r="D22" s="14">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="15" t="str">
+        <v>0,2,3</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,3</v>
+      </c>
+      <c r="H22" t="str">
+        <v>2,3,5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <v>2,3,5</v>
+      </c>
+      <c r="D23" s="14">
+        <v>19</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="15" t="str">
+        <v>0,1,2,3</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,3</v>
+      </c>
+      <c r="H23" t="str">
+        <v>1,4,5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <v>1,4,5</v>
+      </c>
+      <c r="D24" s="14">
+        <v>20</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="15" t="str">
+        <v>0,4</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H24" t="str">
+        <v>2,4,5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <v>2,4,5</v>
+      </c>
+      <c r="D25" s="14">
+        <v>21</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="15" t="str">
+        <v>0,1,4</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,4</v>
+      </c>
+      <c r="H25" t="str">
+        <v>3,4,5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <v>3,4,5</v>
+      </c>
+      <c r="D26" s="14">
+        <v>23</v>
+      </c>
+      <c r="F26" s="15" t="str">
+        <v>0,2,4</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F27" s="15" t="str">
+        <v>0,1,2,4</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,4</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F28" s="15" t="str">
+        <v>0,3,4</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3,4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F29" s="15" t="str">
+        <v>0,1,3,4</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,3,4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F30" s="15" t="str">
+        <v>0,2,3,4</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,3,4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F31" s="15" t="str">
+        <v>0,1,2,3,4</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,3,4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F32" s="15" t="str">
+        <v>0,5</v>
+      </c>
+      <c r="G32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="15" t="str">
+        <v>0,1,5</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,5</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="15" t="str">
+        <v>0,2,5</v>
+      </c>
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,5</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F35" s="15" t="str">
+        <v>0,1,2,5</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F36" s="15" t="str">
+        <v>0,3,5</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3,5</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F37" s="15" t="str">
+        <v>0,1,3,5</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,3,5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F38" s="15" t="str">
+        <v>0,2,3,5</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,3,5</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F39" s="15" t="str">
+        <v>0,1,2,3,5</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,3,5</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F40" s="15" t="str">
+        <v>0,4,5</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4,5</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F41" s="15" t="str">
+        <v>0,1,4,5</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,4,5</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F42" s="15" t="str">
+        <v>0,2,4,5</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,4,5</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F43" s="15" t="str">
+        <v>0,1,2,4,5</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,4,5</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F44" s="15" t="str">
+        <v>0,3,4,5</v>
+      </c>
+      <c r="G44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3,4,5</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F45" s="15" t="str">
+        <v>0,1,3,4,5</v>
+      </c>
+      <c r="G45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,3,4,5</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F46" s="15" t="str">
+        <v>0,2,3,4,5</v>
+      </c>
+      <c r="G46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2,3,4,5</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F47" s="15" t="str">
+        <v>0,1,2,3,4,5</v>
+      </c>
+      <c r="G47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1,2,3,4,5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
interim work on recursive solution
</commit_message>
<xml_diff>
--- a/CH-101 Subsets.xlsx
+++ b/CH-101 Subsets.xlsx
@@ -8,16 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7E6F0-21C1-4D1A-9124-7C23CA058C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC33036-86EE-44CF-9199-9B54B8635AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="5" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="MySIngleFunction" sheetId="7" r:id="rId4"/>
+    <sheet name="RecursiveDetermination" sheetId="8" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_a">RecursiveDetermination!$J$14</definedName>
+    <definedName name="f">_xlfn.LAMBDA(_xlpm.x,_xlpm.s,_xlpm.a,IF(LEN(_xlpm.s)&lt;3,f(_xlpm.x+1,_xlpm.s&amp;"A"),_xlfn.VSTACK(_xlpm.a,_xlpm.s)))</definedName>
+    <definedName name="fx">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, IF(LEN(_xlpm.b)&gt;=3, _xlpm.b, fx(_xlpm.a,_xlpm.a&amp;_xlpm.b)))</definedName>
+    <definedName name="g">_xlfn.LAMBDA(_xlpm.x,IF(_xlpm.x&lt;9,g(_xlpm.x+1),_xlpm.x))</definedName>
+    <definedName name="GCD_RECURSIVE">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, IF(_xlpm.b=0, _xlpm.a, GCD_RECURSIVE(_xlpm.b, MOD(_xlpm.a, _xlpm.b))))</definedName>
+    <definedName name="gx">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, IF(LEN(_xlpm.b)&gt;=3, _xlfn.VSTACK(_xlpm.a,_xlpm.b), gx(_xlpm.a,_xlpm.a&amp;_xlpm.b)))</definedName>
+    <definedName name="h">_xlfn.LAMBDA(_xlpm.x,IF(LEN(_xlpm.x)&lt;3,h(_xlpm.x&amp;_xlpm.x),_xlpm.x))</definedName>
+    <definedName name="hx">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, IF(LEN(_xlpm.b)&gt;=3, _xlfn.VSTACK(_xlpm.a,_xlpm.b), hx(_xlpm.a,_xlpm.a&amp;_xlpm.b)))</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,8 +51,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -52,16 +64,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -115,8 +141,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dddd"/>
+    <numFmt numFmtId="165" formatCode="0;\-0;0;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -254,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -277,14 +304,15 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,6 +675,66 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>3</v>
+    <v>2</v>
+    <v>19</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="argument" t="s"/>
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Organic">
   <a:themeElements>
@@ -931,14 +1019,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1219,14 +1307,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1417,7 +1505,7 @@
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="15" cm="1">
+      <c r="F16" s="13" cm="1">
         <f t="array" ref="F16:F47">_xlfn.REDUCE(
 0,
 B3:B7,
@@ -1472,11 +1560,11 @@
 )</f>
         <v>1,2,3</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>10</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="15" t="str">
+      <c r="F17" s="13" t="str">
         <v>0,1</v>
       </c>
       <c r="G17" s="1" t="str">
@@ -1495,11 +1583,11 @@
       <c r="C18" t="str">
         <v>1,2,4</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>12</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="15" t="str">
+      <c r="F18" s="13" t="str">
         <v>0,2</v>
       </c>
       <c r="G18" s="1" t="str">
@@ -1518,11 +1606,11 @@
       <c r="C19" t="str">
         <v>1,3,4</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>14</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="15" t="str">
+      <c r="F19" s="13" t="str">
         <v>0,1,2</v>
       </c>
       <c r="G19" s="1" t="str">
@@ -1541,11 +1629,11 @@
       <c r="C20" t="str">
         <v>2,3,4</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>15</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="15" t="str">
+      <c r="F20" s="13" t="str">
         <v>0,3</v>
       </c>
       <c r="G20" s="1" t="str">
@@ -1564,11 +1652,11 @@
       <c r="C21" t="str">
         <v>1,2,5</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <v>16</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="15" t="str">
+      <c r="F21" s="13" t="str">
         <v>0,1,3</v>
       </c>
       <c r="G21" s="1" t="str">
@@ -1587,11 +1675,11 @@
       <c r="C22" t="str">
         <v>1,3,5</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <v>18</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="15" t="str">
+      <c r="F22" s="13" t="str">
         <v>0,2,3</v>
       </c>
       <c r="G22" s="1" t="str">
@@ -1610,11 +1698,11 @@
       <c r="C23" t="str">
         <v>2,3,5</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>19</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="15" t="str">
+      <c r="F23" s="13" t="str">
         <v>0,1,2,3</v>
       </c>
       <c r="G23" s="1" t="str">
@@ -1633,11 +1721,11 @@
       <c r="C24" t="str">
         <v>1,4,5</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <v>20</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="15" t="str">
+      <c r="F24" s="13" t="str">
         <v>0,4</v>
       </c>
       <c r="G24" s="1" t="str">
@@ -1656,11 +1744,11 @@
       <c r="C25" t="str">
         <v>2,4,5</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>21</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="15" t="str">
+      <c r="F25" s="13" t="str">
         <v>0,1,4</v>
       </c>
       <c r="G25" s="1" t="str">
@@ -1679,10 +1767,10 @@
       <c r="C26" t="str">
         <v>3,4,5</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <v>23</v>
       </c>
-      <c r="F26" s="15" t="str">
+      <c r="F26" s="13" t="str">
         <v>0,2,4</v>
       </c>
       <c r="G26" s="1" t="str">
@@ -1691,7 +1779,7 @@
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F27" s="15" t="str">
+      <c r="F27" s="13" t="str">
         <v>0,1,2,4</v>
       </c>
       <c r="G27" s="1" t="str">
@@ -1700,7 +1788,7 @@
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F28" s="15" t="str">
+      <c r="F28" s="13" t="str">
         <v>0,3,4</v>
       </c>
       <c r="G28" s="1" t="str">
@@ -1709,7 +1797,7 @@
       </c>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F29" s="15" t="str">
+      <c r="F29" s="13" t="str">
         <v>0,1,3,4</v>
       </c>
       <c r="G29" s="1" t="str">
@@ -1718,7 +1806,7 @@
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F30" s="15" t="str">
+      <c r="F30" s="13" t="str">
         <v>0,2,3,4</v>
       </c>
       <c r="G30" s="1" t="str">
@@ -1727,7 +1815,7 @@
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F31" s="15" t="str">
+      <c r="F31" s="13" t="str">
         <v>0,1,2,3,4</v>
       </c>
       <c r="G31" s="1" t="str">
@@ -1736,7 +1824,7 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F32" s="15" t="str">
+      <c r="F32" s="13" t="str">
         <v>0,5</v>
       </c>
       <c r="G32" s="1" t="str">
@@ -1745,7 +1833,7 @@
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F33" s="15" t="str">
+      <c r="F33" s="13" t="str">
         <v>0,1,5</v>
       </c>
       <c r="G33" s="1" t="str">
@@ -1754,7 +1842,7 @@
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="15" t="str">
+      <c r="F34" s="13" t="str">
         <v>0,2,5</v>
       </c>
       <c r="G34" s="1" t="str">
@@ -1763,7 +1851,7 @@
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F35" s="15" t="str">
+      <c r="F35" s="13" t="str">
         <v>0,1,2,5</v>
       </c>
       <c r="G35" s="1" t="str">
@@ -1772,7 +1860,7 @@
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="15" t="str">
+      <c r="F36" s="13" t="str">
         <v>0,3,5</v>
       </c>
       <c r="G36" s="1" t="str">
@@ -1781,7 +1869,7 @@
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="15" t="str">
+      <c r="F37" s="13" t="str">
         <v>0,1,3,5</v>
       </c>
       <c r="G37" s="1" t="str">
@@ -1790,7 +1878,7 @@
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F38" s="15" t="str">
+      <c r="F38" s="13" t="str">
         <v>0,2,3,5</v>
       </c>
       <c r="G38" s="1" t="str">
@@ -1799,7 +1887,7 @@
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="15" t="str">
+      <c r="F39" s="13" t="str">
         <v>0,1,2,3,5</v>
       </c>
       <c r="G39" s="1" t="str">
@@ -1808,7 +1896,7 @@
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F40" s="15" t="str">
+      <c r="F40" s="13" t="str">
         <v>0,4,5</v>
       </c>
       <c r="G40" s="1" t="str">
@@ -1817,7 +1905,7 @@
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="15" t="str">
+      <c r="F41" s="13" t="str">
         <v>0,1,4,5</v>
       </c>
       <c r="G41" s="1" t="str">
@@ -1826,7 +1914,7 @@
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F42" s="15" t="str">
+      <c r="F42" s="13" t="str">
         <v>0,2,4,5</v>
       </c>
       <c r="G42" s="1" t="str">
@@ -1835,7 +1923,7 @@
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F43" s="15" t="str">
+      <c r="F43" s="13" t="str">
         <v>0,1,2,4,5</v>
       </c>
       <c r="G43" s="1" t="str">
@@ -1844,7 +1932,7 @@
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F44" s="15" t="str">
+      <c r="F44" s="13" t="str">
         <v>0,3,4,5</v>
       </c>
       <c r="G44" s="1" t="str">
@@ -1853,7 +1941,7 @@
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F45" s="15" t="str">
+      <c r="F45" s="13" t="str">
         <v>0,1,3,4,5</v>
       </c>
       <c r="G45" s="1" t="str">
@@ -1862,7 +1950,7 @@
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F46" s="15" t="str">
+      <c r="F46" s="13" t="str">
         <v>0,2,3,4,5</v>
       </c>
       <c r="G46" s="1" t="str">
@@ -1871,7 +1959,7 @@
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F47" s="15" t="str">
+      <c r="F47" s="13" t="str">
         <v>0,1,2,3,4,5</v>
       </c>
       <c r="G47" s="1" t="str">
@@ -1911,14 +1999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="2:9" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -2424,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10E6EC7-929D-4B79-9534-5782F0C92B71}">
   <dimension ref="B1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L8:L9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,14 +2529,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="H1" s="13" t="s">
+      <c r="C1" s="15"/>
+      <c r="H1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="2:14" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -2639,7 +2727,7 @@
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="15" cm="1">
+      <c r="F16" s="13" cm="1">
         <f t="array" ref="F16:F47">_xlfn.REDUCE(
 0,
 B3:B7,
@@ -2714,11 +2802,11 @@
 )</f>
         <v>1,2,3</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>10</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="15" t="str">
+      <c r="F17" s="13" t="str">
         <v>0,1</v>
       </c>
       <c r="G17" s="1" t="str">
@@ -2749,11 +2837,11 @@
       <c r="C18" t="str">
         <v>1,2,4</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>12</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="15" t="str">
+      <c r="F18" s="13" t="str">
         <v>0,2</v>
       </c>
       <c r="G18" s="1" t="str">
@@ -2784,11 +2872,11 @@
       <c r="C19" t="str">
         <v>1,3,4</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>14</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="15" t="str">
+      <c r="F19" s="13" t="str">
         <v>0,1,2</v>
       </c>
       <c r="G19" s="1" t="str">
@@ -2819,11 +2907,11 @@
       <c r="C20" t="str">
         <v>2,3,4</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>15</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="15" t="str">
+      <c r="F20" s="13" t="str">
         <v>0,3</v>
       </c>
       <c r="G20" s="1" t="str">
@@ -2854,11 +2942,11 @@
       <c r="C21" t="str">
         <v>1,2,5</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <v>16</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="15" t="str">
+      <c r="F21" s="13" t="str">
         <v>0,1,3</v>
       </c>
       <c r="G21" s="1" t="str">
@@ -2889,11 +2977,11 @@
       <c r="C22" t="str">
         <v>1,3,5</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <v>18</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="15" t="str">
+      <c r="F22" s="13" t="str">
         <v>0,2,3</v>
       </c>
       <c r="G22" s="1" t="str">
@@ -2924,11 +3012,11 @@
       <c r="C23" t="str">
         <v>2,3,5</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>19</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="15" t="str">
+      <c r="F23" s="13" t="str">
         <v>0,1,2,3</v>
       </c>
       <c r="G23" s="1" t="str">
@@ -2959,11 +3047,11 @@
       <c r="C24" t="str">
         <v>1,4,5</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <v>20</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="15" t="str">
+      <c r="F24" s="13" t="str">
         <v>0,4</v>
       </c>
       <c r="G24" s="1" t="str">
@@ -2994,11 +3082,11 @@
       <c r="C25" t="str">
         <v>2,4,5</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>21</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="15" t="str">
+      <c r="F25" s="13" t="str">
         <v>0,1,4</v>
       </c>
       <c r="G25" s="1" t="str">
@@ -3029,10 +3117,10 @@
       <c r="C26" t="str">
         <v>3,4,5</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <v>23</v>
       </c>
-      <c r="F26" s="15" t="str">
+      <c r="F26" s="13" t="str">
         <v>0,2,4</v>
       </c>
       <c r="G26" s="1" t="str">
@@ -3041,7 +3129,7 @@
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F27" s="15" t="str">
+      <c r="F27" s="13" t="str">
         <v>0,1,2,4</v>
       </c>
       <c r="G27" s="1" t="str">
@@ -3050,7 +3138,7 @@
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F28" s="15" t="str">
+      <c r="F28" s="13" t="str">
         <v>0,3,4</v>
       </c>
       <c r="G28" s="1" t="str">
@@ -3059,7 +3147,7 @@
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F29" s="15" t="str">
+      <c r="F29" s="13" t="str">
         <v>0,1,3,4</v>
       </c>
       <c r="G29" s="1" t="str">
@@ -3068,7 +3156,7 @@
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F30" s="15" t="str">
+      <c r="F30" s="13" t="str">
         <v>0,2,3,4</v>
       </c>
       <c r="G30" s="1" t="str">
@@ -3077,7 +3165,7 @@
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F31" s="15" t="str">
+      <c r="F31" s="13" t="str">
         <v>0,1,2,3,4</v>
       </c>
       <c r="G31" s="1" t="str">
@@ -3086,7 +3174,7 @@
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="F32" s="15" t="str">
+      <c r="F32" s="13" t="str">
         <v>0,5</v>
       </c>
       <c r="G32" s="1" t="str">
@@ -3095,7 +3183,7 @@
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F33" s="15" t="str">
+      <c r="F33" s="13" t="str">
         <v>0,1,5</v>
       </c>
       <c r="G33" s="1" t="str">
@@ -3104,7 +3192,7 @@
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="15" t="str">
+      <c r="F34" s="13" t="str">
         <v>0,2,5</v>
       </c>
       <c r="G34" s="1" t="str">
@@ -3113,7 +3201,7 @@
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F35" s="15" t="str">
+      <c r="F35" s="13" t="str">
         <v>0,1,2,5</v>
       </c>
       <c r="G35" s="1" t="str">
@@ -3122,7 +3210,7 @@
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="15" t="str">
+      <c r="F36" s="13" t="str">
         <v>0,3,5</v>
       </c>
       <c r="G36" s="1" t="str">
@@ -3131,7 +3219,7 @@
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F37" s="15" t="str">
+      <c r="F37" s="13" t="str">
         <v>0,1,3,5</v>
       </c>
       <c r="G37" s="1" t="str">
@@ -3140,7 +3228,7 @@
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F38" s="15" t="str">
+      <c r="F38" s="13" t="str">
         <v>0,2,3,5</v>
       </c>
       <c r="G38" s="1" t="str">
@@ -3149,7 +3237,7 @@
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F39" s="15" t="str">
+      <c r="F39" s="13" t="str">
         <v>0,1,2,3,5</v>
       </c>
       <c r="G39" s="1" t="str">
@@ -3158,7 +3246,7 @@
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F40" s="15" t="str">
+      <c r="F40" s="13" t="str">
         <v>0,4,5</v>
       </c>
       <c r="G40" s="1" t="str">
@@ -3167,7 +3255,7 @@
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F41" s="15" t="str">
+      <c r="F41" s="13" t="str">
         <v>0,1,4,5</v>
       </c>
       <c r="G41" s="1" t="str">
@@ -3176,7 +3264,7 @@
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F42" s="15" t="str">
+      <c r="F42" s="13" t="str">
         <v>0,2,4,5</v>
       </c>
       <c r="G42" s="1" t="str">
@@ -3185,7 +3273,7 @@
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F43" s="15" t="str">
+      <c r="F43" s="13" t="str">
         <v>0,1,2,4,5</v>
       </c>
       <c r="G43" s="1" t="str">
@@ -3194,7 +3282,7 @@
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F44" s="15" t="str">
+      <c r="F44" s="13" t="str">
         <v>0,3,4,5</v>
       </c>
       <c r="G44" s="1" t="str">
@@ -3203,7 +3291,7 @@
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F45" s="15" t="str">
+      <c r="F45" s="13" t="str">
         <v>0,1,3,4,5</v>
       </c>
       <c r="G45" s="1" t="str">
@@ -3212,7 +3300,7 @@
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F46" s="15" t="str">
+      <c r="F46" s="13" t="str">
         <v>0,2,3,4,5</v>
       </c>
       <c r="G46" s="1" t="str">
@@ -3221,7 +3309,7 @@
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F47" s="15" t="str">
+      <c r="F47" s="13" t="str">
         <v>0,1,2,3,4,5</v>
       </c>
       <c r="G47" s="1" t="str">
@@ -3238,4 +3326,359 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C1E872-474F-4BFF-AFB2-C20E12A1B771}">
+  <dimension ref="B1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="18.75" customWidth="1"/>
+    <col min="9" max="9" width="15.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.375" customWidth="1"/>
+    <col min="11" max="11" width="19.375" customWidth="1"/>
+    <col min="12" max="12" width="17.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="H1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10"/>
+      <c r="H10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D16" s="1"/>
+      <c r="E16" s="14" t="str" cm="1">
+        <f t="array" ref="E16">_xlfn.LET(
+_xlpm.h,_xlfn.LAMBDA(_xlpm.x,IF(_xlpm.x&lt;5,h(_xlpm.x+3),_xlpm.x)),
+_xlpm.h(1)
+)</f>
+        <v>4444</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="14" cm="1">
+        <f t="array" ref="G16">g(1)</f>
+        <v>9</v>
+      </c>
+      <c r="I16" s="6" t="e" cm="1" vm="1">
+        <f t="array" ref="I16">_xlfn.LAMBDA(_xlpm.x,_xlpm.s,IF(LEN(_xlpm.s)&lt;3,f(_xlpm.x+1,_xlpm.s&amp;_xlpm.x+1),_xlfn.VSTACK(_a,_xlpm.s)))(1,"")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" t="str" cm="1">
+        <f t="array" ref="K16">h("1")</f>
+        <v>1111</v>
+      </c>
+      <c r="L16">
+        <f>LEN(K16)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" t="e" cm="1" vm="1">
+        <f t="array" ref="H18">f(1,"0","")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I18" s="6" t="e" cm="1" vm="1">
+        <f t="array" ref="I18">f(1,"","0")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H27" cm="1">
+        <f t="array" ref="H27">GCD_RECURSIVE(48, 18)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H30" t="str" cm="1">
+        <f t="array" ref="H30">fx("3", "1")</f>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H31" t="str" cm="1">
+        <f t="array" ref="H31:H32">gx("3","3")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H32" t="str">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H34" cm="1">
+        <f t="array" ref="H34:H35">hx(3,"3")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H35" t="str">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>